<commit_message>
Added test execution report for OpenCart
</commit_message>
<xml_diff>
--- a/OpenCart-ManualTesting-main/OpenCart-Test Scenarios.xlsx
+++ b/OpenCart-ManualTesting-main/OpenCart-Test Scenarios.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -326,13 +326,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
@@ -403,20 +403,20 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,8 +637,8 @@
   </sheetPr>
   <dimension ref="A2:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -648,72 +648,72 @@
     <col min="3" max="3" width="22.90625" customWidth="1"/>
     <col min="4" max="4" width="78.08984375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>46024</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>46027</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>